<commit_message>
API Get list product and post
</commit_message>
<xml_diff>
--- a/document/Database.xlsx
+++ b/document/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Monhoc\CDWeb\chuyen-de-web\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBBA67F-42AC-494F-B87D-ECA74FABBCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151FF0FC-70C6-41F4-BF38-C1441604EC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -321,10 +321,10 @@
     <t>View: 300</t>
   </si>
   <si>
-    <t>Taxomony</t>
-  </si>
-  <si>
     <t>Đổi product_id thành post_id và wishlist thành favorite</t>
+  </si>
+  <si>
+    <t>Taxomony: 50</t>
   </si>
 </sst>
 </file>
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C16"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -975,7 +975,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="I2" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J2" s="29"/>
       <c r="K2" s="30"/>
@@ -1120,7 +1120,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="E8" s="42" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F8" s="42"/>
       <c r="G8" s="42"/>

</xml_diff>

<commit_message>
Update database and taxomony API
</commit_message>
<xml_diff>
--- a/document/Database.xlsx
+++ b/document/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Monhoc\CDWeb\chuyen-de-web\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925CDF9B-FFA4-409C-8460-EB12E89D514B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93D9C64-17E8-46D6-A85B-5DCD495380E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -541,6 +541,46 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,46 +635,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -944,26 +944,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="E1" s="28" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="E1" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="I1" s="40" t="s">
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="I1" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="M1" s="36" t="s">
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -972,11 +972,11 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="I2" s="46" t="s">
+      <c r="I2" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="47"/>
-      <c r="K2" s="48"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="31"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
@@ -1098,11 +1098,11 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
       <c r="M7" s="13" t="s">
         <v>57</v>
       </c>
@@ -1117,16 +1117,16 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="I8" s="41" t="s">
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="I8" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
       <c r="M8" s="13" t="s">
         <v>58</v>
       </c>
@@ -1311,13 +1311,13 @@
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="49" t="s">
+      <c r="E14" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="49" t="s">
+      <c r="G14" s="18" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1356,16 +1356,16 @@
       <c r="G16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="42" t="s">
+      <c r="I16" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="43"/>
-      <c r="K16" s="44"/>
-      <c r="M16" s="37" t="s">
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="M16" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E17" s="4" t="s">
@@ -1452,16 +1452,16 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="32"/>
-      <c r="E21" s="33" t="s">
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="E21" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
       <c r="I21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1544,11 +1544,11 @@
       <c r="G24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="45" t="s">
+      <c r="I24" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -1601,11 +1601,11 @@
       <c r="K26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="38" t="s">
+      <c r="M26" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I27" s="12" t="s">
@@ -1642,16 +1642,16 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="E29" s="39" t="s">
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="E29" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
       <c r="I29" s="12" t="s">
         <v>54</v>
       </c>
@@ -1868,11 +1868,11 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="34"/>
       <c r="E37" s="8" t="s">
         <v>48</v>
       </c>
@@ -1882,11 +1882,11 @@
       <c r="G37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I37" s="39" t="s">
+      <c r="I37" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="J37" s="39"/>
-      <c r="K37" s="39"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
@@ -1984,11 +1984,11 @@
       <c r="K42" s="8"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E43" s="28" t="s">
+      <c r="E43" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
       <c r="I43" s="8" t="s">
         <v>13</v>
       </c>
@@ -2032,11 +2032,11 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="23"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="37"/>
       <c r="E46" s="3" t="s">
         <v>76</v>
       </c>
@@ -2093,11 +2093,11 @@
       <c r="C50" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="34" t="s">
+      <c r="E50" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
@@ -2233,11 +2233,11 @@
       <c r="C59" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="35" t="s">
+      <c r="E59" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="F59" s="35"/>
-      <c r="G59" s="35"/>
+      <c r="F59" s="49"/>
+      <c r="G59" s="49"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
@@ -2303,11 +2303,11 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="24" t="s">
+      <c r="A65" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="25"/>
-      <c r="C65" s="26"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="40"/>
       <c r="E65" s="17" t="s">
         <v>94</v>
       </c>
@@ -2369,16 +2369,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I2:K2"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A65:C65"/>
@@ -2392,6 +2382,16 @@
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E59:G59"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I2:K2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Filter post and taxomony
</commit_message>
<xml_diff>
--- a/document/Database.xlsx
+++ b/document/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Monhoc\CDWeb\chuyen-de-web\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93D9C64-17E8-46D6-A85B-5DCD495380E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E555278E-6EF2-4FD7-8C4F-E8C7E23327F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -542,6 +542,60 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -579,60 +633,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -925,7 +925,7 @@
   <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -944,26 +944,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="E1" s="42" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="E1" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="I1" s="23" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="I1" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="M1" s="19" t="s">
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="M1" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -972,11 +972,11 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="49"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
@@ -1098,11 +1098,11 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="M7" s="13" t="s">
         <v>57</v>
       </c>
@@ -1117,16 +1117,16 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="I8" s="24" t="s">
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="I8" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
       <c r="M8" s="13" t="s">
         <v>58</v>
       </c>
@@ -1356,16 +1356,16 @@
       <c r="G16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="25" t="s">
+      <c r="I16" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
-      <c r="M16" s="20" t="s">
+      <c r="J16" s="44"/>
+      <c r="K16" s="45"/>
+      <c r="M16" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E17" s="4" t="s">
@@ -1452,16 +1452,16 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="E21" s="47" t="s">
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="E21" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
       <c r="I21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1544,11 +1544,11 @@
       <c r="G24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="28" t="s">
+      <c r="I24" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -1601,11 +1601,11 @@
       <c r="K26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="21" t="s">
+      <c r="M26" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I27" s="12" t="s">
@@ -1642,16 +1642,16 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="E29" s="22" t="s">
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="E29" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
       <c r="I29" s="12" t="s">
         <v>54</v>
       </c>
@@ -1868,11 +1868,6 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="34"/>
       <c r="E37" s="8" t="s">
         <v>48</v>
       </c>
@@ -1882,16 +1877,18 @@
       <c r="G37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I37" s="22" t="s">
+      <c r="I37" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
+      <c r="A38" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
       <c r="E38" s="8" t="s">
         <v>49</v>
       </c>
@@ -1906,15 +1903,9 @@
       <c r="K38" s="8"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
       <c r="I39" s="8" t="s">
         <v>0</v>
       </c>
@@ -1927,7 +1918,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>2</v>
@@ -1947,7 +1938,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>2</v>
@@ -1967,10 +1958,10 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>4</v>
@@ -1984,11 +1975,20 @@
       <c r="K42" s="8"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E43" s="42" t="s">
+      <c r="A43" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
       <c r="I43" s="8" t="s">
         <v>13</v>
       </c>
@@ -2032,11 +2032,11 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="37"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="24"/>
       <c r="E46" s="3" t="s">
         <v>76</v>
       </c>
@@ -2093,11 +2093,11 @@
       <c r="C50" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="48" t="s">
+      <c r="E50" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
@@ -2233,11 +2233,11 @@
       <c r="C59" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="49" t="s">
+      <c r="E59" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
@@ -2303,11 +2303,11 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="38" t="s">
+      <c r="A65" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="39"/>
-      <c r="C65" s="40"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="27"/>
       <c r="E65" s="17" t="s">
         <v>94</v>
       </c>
@@ -2369,7 +2369,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="A38:C38"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A65:C65"/>
     <mergeCell ref="A7:C7"/>
@@ -2382,16 +2392,6 @@
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E59:G59"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I2:K2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UserAccount and User API
</commit_message>
<xml_diff>
--- a/document/Database.xlsx
+++ b/document/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Monhoc\CDWeb\chuyen-de-web\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E555278E-6EF2-4FD7-8C4F-E8C7E23327F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDB71DD-BA52-429B-8B13-3F6411781403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="102">
   <si>
     <t>id</t>
   </si>
@@ -322,6 +322,15 @@
   </si>
   <si>
     <t>Taxomony: 50</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>birthday</t>
   </si>
 </sst>
 </file>
@@ -542,6 +551,45 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,45 +642,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -924,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -944,26 +953,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="E1" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="I1" s="41" t="s">
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="I1" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="M1" s="37" t="s">
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -972,11 +981,11 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="48"/>
-      <c r="K2" s="49"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="31"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
@@ -1098,11 +1107,11 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
       <c r="M7" s="13" t="s">
         <v>57</v>
       </c>
@@ -1117,16 +1126,16 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="I8" s="42" t="s">
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="I8" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
       <c r="M8" s="13" t="s">
         <v>58</v>
       </c>
@@ -1303,14 +1312,12 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C14" s="2"/>
       <c r="E14" s="18" t="s">
         <v>23</v>
       </c>
@@ -1323,10 +1330,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2"/>
       <c r="E15" s="4" t="s">
@@ -1339,13 +1346,13 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>13</v>
@@ -1356,18 +1363,25 @@
       <c r="G16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="43" t="s">
+      <c r="I16" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="44"/>
-      <c r="K16" s="45"/>
-      <c r="M16" s="38" t="s">
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="M16" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="E17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1383,6 +1397,15 @@
       <c r="O17" s="14"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E18" s="4" t="s">
         <v>15</v>
       </c>
@@ -1452,16 +1475,16 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="E21" s="34" t="s">
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="E21" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
       <c r="I21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1544,11 +1567,11 @@
       <c r="G24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="46" t="s">
+      <c r="I24" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -1601,11 +1624,11 @@
       <c r="K26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="39" t="s">
+      <c r="M26" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="N26" s="39"/>
-      <c r="O26" s="39"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I27" s="12" t="s">
@@ -1642,16 +1665,16 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="E29" s="40" t="s">
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="E29" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
       <c r="I29" s="12" t="s">
         <v>54</v>
       </c>
@@ -1877,18 +1900,18 @@
       <c r="G37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I37" s="40" t="s">
+      <c r="I37" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="34"/>
       <c r="E38" s="8" t="s">
         <v>49</v>
       </c>
@@ -1984,11 +2007,11 @@
       <c r="C43" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="29" t="s">
+      <c r="E43" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
       <c r="I43" s="8" t="s">
         <v>13</v>
       </c>
@@ -2032,11 +2055,11 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="24"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="37"/>
       <c r="E46" s="3" t="s">
         <v>76</v>
       </c>
@@ -2093,11 +2116,11 @@
       <c r="C50" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="35" t="s">
+      <c r="E50" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
@@ -2233,11 +2256,11 @@
       <c r="C59" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="36" t="s">
+      <c r="E59" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
+      <c r="F59" s="49"/>
+      <c r="G59" s="49"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
@@ -2303,11 +2326,11 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="26"/>
-      <c r="C65" s="27"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="40"/>
       <c r="E65" s="17" t="s">
         <v>94</v>
       </c>
@@ -2369,16 +2392,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I2:K2"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A65:C65"/>
@@ -2392,6 +2405,16 @@
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E59:G59"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I2:K2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update DB and fix loadUser
</commit_message>
<xml_diff>
--- a/document/Database.xlsx
+++ b/document/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Monhoc\CDWeb\chuyen-de-web\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDB71DD-BA52-429B-8B13-3F6411781403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661AF001-5461-415B-92A4-4CAE74CC3F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="100">
   <si>
     <t>id</t>
   </si>
@@ -210,15 +210,6 @@
     <t>image</t>
   </si>
   <si>
-    <t>is_default</t>
-  </si>
-  <si>
-    <t>bit</t>
-  </si>
-  <si>
-    <t>default: false</t>
-  </si>
-  <si>
     <t>star</t>
   </si>
   <si>
@@ -331,6 +322,9 @@
   </si>
   <si>
     <t>birthday</t>
+  </si>
+  <si>
+    <t>priority</t>
   </si>
 </sst>
 </file>
@@ -551,6 +545,60 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -588,60 +636,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -934,7 +928,7 @@
   <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I8" sqref="I8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -953,26 +947,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="E1" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="I1" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="M1" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
+      <c r="A1" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="E1" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="I1" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="M1" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -981,11 +975,11 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="I2" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="I2" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="48"/>
+      <c r="K2" s="49"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
@@ -1033,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -1100,23 +1094,23 @@
         <v>56</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
+      <c r="A7" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="M7" s="13" t="s">
         <v>57</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="O7" s="13" t="s">
         <v>4</v>
@@ -1126,21 +1120,21 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="E8" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="I8" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="E8" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="I8" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
       <c r="M8" s="13" t="s">
         <v>58</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="O8" s="13" t="s">
         <v>4</v>
@@ -1199,13 +1193,13 @@
         <v>4</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="O10" s="13" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -1256,7 +1250,7 @@
         <v>22</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>4</v>
@@ -1312,17 +1306,17 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C14" s="2"/>
       <c r="E14" s="18" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>4</v>
@@ -1330,7 +1324,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
@@ -1363,16 +1357,16 @@
       <c r="G16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
-      <c r="M16" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
+      <c r="I16" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="44"/>
+      <c r="K16" s="45"/>
+      <c r="M16" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -1448,7 +1442,7 @@
         <v>1</v>
       </c>
       <c r="N19" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="O19" s="14" t="s">
         <v>4</v>
@@ -1468,23 +1462,23 @@
         <v>60</v>
       </c>
       <c r="N20" s="14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="O20" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="E21" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
+      <c r="A21" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="E21" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
       <c r="I21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1550,7 +1544,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>9</v>
@@ -1567,15 +1561,15 @@
       <c r="G24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
+      <c r="I24" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>9</v>
@@ -1624,11 +1618,11 @@
       <c r="K26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
+      <c r="M26" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I27" s="12" t="s">
@@ -1665,16 +1659,16 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="E29" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
+      <c r="A29" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="E29" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
       <c r="I29" s="12" t="s">
         <v>54</v>
       </c>
@@ -1702,7 +1696,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="I30" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>2</v>
@@ -1799,7 +1793,7 @@
         <v>23</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>4</v>
@@ -1832,7 +1826,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>9</v>
@@ -1900,18 +1894,18 @@
       <c r="G37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I37" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
+      <c r="I37" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="33"/>
-      <c r="C38" s="34"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
       <c r="E38" s="8" t="s">
         <v>49</v>
       </c>
@@ -1970,7 +1964,7 @@
         <v>4</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>2</v>
@@ -2007,11 +2001,11 @@
       <c r="C43" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
+      <c r="E43" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
       <c r="I43" s="8" t="s">
         <v>13</v>
       </c>
@@ -2055,13 +2049,13 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="37"/>
+      <c r="A46" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="24"/>
       <c r="E46" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>2</v>
@@ -2075,7 +2069,7 @@
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="E47" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>2</v>
@@ -2116,11 +2110,11 @@
       <c r="C50" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
+      <c r="E50" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
@@ -2141,7 +2135,7 @@
         <v>43</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C52" s="7"/>
       <c r="E52" s="1" t="s">
@@ -2166,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>4</v>
@@ -2213,7 +2207,7 @@
         <v>22</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>4</v>
@@ -2256,11 +2250,11 @@
       <c r="C59" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
+      <c r="E59" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
@@ -2319,20 +2313,20 @@
         <v>23</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G64" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B65" s="39"/>
-      <c r="C65" s="40"/>
+      <c r="A65" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="26"/>
+      <c r="C65" s="27"/>
       <c r="E65" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F65" s="17" t="s">
         <v>16</v>
@@ -2392,6 +2386,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I2:K2"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A65:C65"/>
@@ -2405,16 +2409,6 @@
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E59:G59"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I2:K2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update DB type post, wishlist to favorite
</commit_message>
<xml_diff>
--- a/document/Database.xlsx
+++ b/document/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Monhoc\CDWeb\chuyen-de-web\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661AF001-5461-415B-92A4-4CAE74CC3F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1C8972-B3FB-4170-8963-93D3548BCAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="99">
   <si>
     <t>id</t>
   </si>
@@ -261,9 +261,6 @@
     <t>Attribute: 150</t>
   </si>
   <si>
-    <t>Wishlist: 100</t>
-  </si>
-  <si>
     <t>Cart: 100</t>
   </si>
   <si>
@@ -309,9 +306,6 @@
     <t>View: 300</t>
   </si>
   <si>
-    <t>Đổi product_id thành post_id và wishlist thành favorite</t>
-  </si>
-  <si>
     <t>Taxomony: 50</t>
   </si>
   <si>
@@ -325,6 +319,9 @@
   </si>
   <si>
     <t>priority</t>
+  </si>
+  <si>
+    <t>Favorite: 300</t>
   </si>
 </sst>
 </file>
@@ -545,6 +542,45 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -597,45 +633,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -927,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:K8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -947,26 +944,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="E1" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="I1" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="M1" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="I1" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -975,11 +972,9 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="I2" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="J2" s="48"/>
-      <c r="K2" s="49"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="31"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
@@ -1042,7 +1037,7 @@
         <v>4</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>2</v>
@@ -1101,11 +1096,11 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
       <c r="M7" s="13" t="s">
         <v>57</v>
       </c>
@@ -1120,16 +1115,16 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="E8" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="I8" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
+      <c r="E8" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="I8" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
       <c r="M8" s="13" t="s">
         <v>58</v>
       </c>
@@ -1193,7 +1188,7 @@
         <v>4</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N10" s="15" t="s">
         <v>2</v>
@@ -1250,7 +1245,7 @@
         <v>22</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>4</v>
@@ -1306,10 +1301,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C14" s="2"/>
       <c r="E14" s="18" t="s">
@@ -1324,7 +1319,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
@@ -1357,16 +1352,16 @@
       <c r="G16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="J16" s="44"/>
-      <c r="K16" s="45"/>
-      <c r="M16" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
+      <c r="I16" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="M16" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -1462,23 +1457,23 @@
         <v>60</v>
       </c>
       <c r="N20" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O20" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="E21" s="34" t="s">
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="E21" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
       <c r="I21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1544,7 +1539,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>9</v>
@@ -1561,15 +1556,15 @@
       <c r="G24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
+      <c r="I24" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>9</v>
@@ -1618,11 +1613,11 @@
       <c r="K26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="N26" s="39"/>
-      <c r="O26" s="39"/>
+      <c r="M26" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I27" s="12" t="s">
@@ -1659,16 +1654,16 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="E29" s="40" t="s">
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="E29" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
       <c r="I29" s="12" t="s">
         <v>54</v>
       </c>
@@ -1696,7 +1691,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="I30" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>2</v>
@@ -1826,7 +1821,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>9</v>
@@ -1894,18 +1889,18 @@
       <c r="G37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I37" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40"/>
+      <c r="I37" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="34"/>
       <c r="E38" s="8" t="s">
         <v>49</v>
       </c>
@@ -2001,11 +1996,11 @@
       <c r="C43" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="29" t="s">
+      <c r="E43" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
       <c r="I43" s="8" t="s">
         <v>13</v>
       </c>
@@ -2049,11 +2044,11 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="24"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="37"/>
       <c r="E46" s="3" t="s">
         <v>73</v>
       </c>
@@ -2110,11 +2105,11 @@
       <c r="C50" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="35" t="s">
+      <c r="E50" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
@@ -2135,7 +2130,7 @@
         <v>43</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C52" s="7"/>
       <c r="E52" s="1" t="s">
@@ -2207,7 +2202,7 @@
         <v>22</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>4</v>
@@ -2250,11 +2245,11 @@
       <c r="C59" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
+      <c r="E59" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="F59" s="49"/>
+      <c r="G59" s="49"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
@@ -2313,20 +2308,20 @@
         <v>23</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G64" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="26"/>
-      <c r="C65" s="27"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="40"/>
       <c r="E65" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F65" s="17" t="s">
         <v>16</v>
@@ -2386,16 +2381,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I2:K2"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A65:C65"/>
@@ -2409,6 +2394,16 @@
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E59:G59"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I2:K2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add feedback to DB
</commit_message>
<xml_diff>
--- a/document/Database.xlsx
+++ b/document/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Monhoc\CDWeb\chuyen-de-web\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1C8972-B3FB-4170-8963-93D3548BCAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3265ED5-14F0-4B62-930B-4AAD434A0674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="104">
   <si>
     <t>id</t>
   </si>
@@ -322,6 +322,21 @@
   </si>
   <si>
     <t>Favorite: 300</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>nvarchar(200)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -522,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -542,6 +557,60 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,60 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -941,45 +957,55 @@
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="E1" s="42" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="E1" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="I1" s="23" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="I1" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="M1" s="19" t="s">
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="M1" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="Q1" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="49"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,8 +1042,17 @@
       <c r="O3" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1054,8 +1089,17 @@
       <c r="O4" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1083,8 +1127,17 @@
       <c r="O5" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="M6" s="13" t="s">
         <v>56</v>
       </c>
@@ -1094,13 +1147,22 @@
       <c r="O6" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
+      <c r="Q6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="M7" s="13" t="s">
         <v>57</v>
       </c>
@@ -1110,21 +1172,30 @@
       <c r="O7" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="I8" s="24" t="s">
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="I8" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
       <c r="M8" s="13" t="s">
         <v>58</v>
       </c>
@@ -1134,8 +1205,17 @@
       <c r="O8" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q8" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="R8" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" s="50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1160,8 +1240,15 @@
       <c r="O9" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1197,7 +1284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1233,7 +1320,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1265,7 +1352,7 @@
       </c>
       <c r="O12" s="13"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1299,7 +1386,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>94</v>
       </c>
@@ -1317,7 +1404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>96</v>
       </c>
@@ -1333,7 +1420,7 @@
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1352,16 +1439,16 @@
       <c r="G16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="25" t="s">
+      <c r="I16" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
-      <c r="M16" s="20" t="s">
+      <c r="J16" s="44"/>
+      <c r="K16" s="45"/>
+      <c r="M16" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -1464,16 +1551,16 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="E21" s="47" t="s">
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="E21" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
       <c r="I21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1556,11 +1643,11 @@
       <c r="G24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="28" t="s">
+      <c r="I24" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -1613,11 +1700,11 @@
       <c r="K26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="21" t="s">
+      <c r="M26" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I27" s="12" t="s">
@@ -1654,16 +1741,16 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="E29" s="22" t="s">
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="E29" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
       <c r="I29" s="12" t="s">
         <v>54</v>
       </c>
@@ -1889,18 +1976,18 @@
       <c r="G37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I37" s="22" t="s">
+      <c r="I37" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="33"/>
-      <c r="C38" s="34"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
       <c r="E38" s="8" t="s">
         <v>49</v>
       </c>
@@ -1996,11 +2083,11 @@
       <c r="C43" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="42" t="s">
+      <c r="E43" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
       <c r="I43" s="8" t="s">
         <v>13</v>
       </c>
@@ -2044,11 +2131,11 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="37"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="24"/>
       <c r="E46" s="3" t="s">
         <v>73</v>
       </c>
@@ -2105,11 +2192,11 @@
       <c r="C50" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E50" s="48" t="s">
+      <c r="E50" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
@@ -2245,11 +2332,11 @@
       <c r="C59" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="49" t="s">
+      <c r="E59" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
@@ -2315,11 +2402,11 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="38" t="s">
+      <c r="A65" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="39"/>
-      <c r="C65" s="40"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="27"/>
       <c r="E65" s="17" t="s">
         <v>90</v>
       </c>
@@ -2380,7 +2467,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I2:K2"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A65:C65"/>
@@ -2394,16 +2492,6 @@
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E59:G59"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I2:K2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>